<commit_message>
02-05-2018 : bugfix : clsProcess->AttdProcess-> Sanction overtime on WO also considered if employee did not come.
</commit_message>
<xml_diff>
--- a/upload_template/BulkSanction_Upload.xlsx
+++ b/upload_template/BulkSanction_Upload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance-Kosi\Attendance - Okhla\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>InTime</t>
   </si>
@@ -39,16 +39,28 @@
     <t>TPAHours</t>
   </si>
   <si>
-    <t>2017-12-01</t>
-  </si>
-  <si>
-    <t>AA</t>
+    <t>2018-04-04</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>2018-04-05</t>
+  </si>
+  <si>
+    <t>2018-04-06</t>
+  </si>
+  <si>
+    <t>2018-04-07</t>
+  </si>
+  <si>
+    <t>20:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,8 +107,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -398,7 +438,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,34 +469,65 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>20005890</v>
+        <v>100234</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
+      <c r="A3">
+        <v>100234</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
+      <c r="A4">
+        <v>100234</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
+      <c r="A5">
+        <v>100234</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>

</xml_diff>